<commit_message>
Objective 3 scaled (not %100 sure)
</commit_message>
<xml_diff>
--- a/data2.xlsx
+++ b/data2.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66129CC4-14F4-6743-8824-2D08A0056293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="32200" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,12 +20,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Yazar</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -32,7 +33,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Yazar:</t>
         </r>
@@ -41,14 +42,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Number of time periods</t>
         </r>
       </text>
     </comment>
-    <comment ref="B2" authorId="0" shapeId="0">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -56,14 +57,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Yazar:
 number of commodities</t>
         </r>
       </text>
     </comment>
-    <comment ref="C2" authorId="0" shapeId="0">
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -71,7 +72,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Yazar:</t>
         </r>
@@ -80,14 +81,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Number of nodes</t>
         </r>
       </text>
     </comment>
-    <comment ref="A3" authorId="0" shapeId="0">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -95,7 +96,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Yazar:</t>
         </r>
@@ -104,7 +105,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 First column: Origin Node
@@ -112,7 +113,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C3" authorId="0" shapeId="0">
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -120,7 +121,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Yazar:</t>
         </r>
@@ -129,14 +130,47 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 B</t>
         </r>
       </text>
     </comment>
-    <comment ref="D3" authorId="0" shapeId="0">
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yazar:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sikt</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -144,7 +178,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Yazar:</t>
         </r>
@@ -153,14 +187,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Sikt</t>
+djkt</t>
         </r>
       </text>
     </comment>
-    <comment ref="G3" authorId="0" shapeId="0">
+    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -168,7 +202,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Yazar:</t>
         </r>
@@ -177,14 +211,15 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-djkt</t>
+Cijkt
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="J3" authorId="0" shapeId="0">
+    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -192,7 +227,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Yazar:</t>
         </r>
@@ -201,15 +236,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Cijkt
-</t>
+Uijt</t>
         </r>
       </text>
     </comment>
-    <comment ref="M3" authorId="0" shapeId="0">
+    <comment ref="P3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -217,7 +251,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Yazar:</t>
         </r>
@@ -226,14 +260,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Uijt</t>
+blocked</t>
         </r>
       </text>
     </comment>
-    <comment ref="P3" authorId="0" shapeId="0">
+    <comment ref="S3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -241,7 +275,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Yazar:</t>
         </r>
@@ -250,14 +284,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-blocked</t>
+bt</t>
         </r>
       </text>
     </comment>
-    <comment ref="S3" authorId="0" shapeId="0">
+    <comment ref="T3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -265,7 +299,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Yazar:</t>
         </r>
@@ -274,14 +308,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 bt</t>
         </r>
       </text>
     </comment>
-    <comment ref="T3" authorId="0" shapeId="0">
+    <comment ref="V3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -289,7 +323,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Yazar:</t>
         </r>
@@ -298,31 +332,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-bt</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="V3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Yazar:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 aij</t>
@@ -342,8 +352,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -356,13 +366,26 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -708,16 +731,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="X5" sqref="X5"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1</v>
       </c>
@@ -785,7 +808,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>3</v>
       </c>
@@ -853,7 +876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -864,13 +887,13 @@
         <v>0</v>
       </c>
       <c r="D3" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E3" s="2">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F3" s="2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -921,7 +944,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -932,13 +955,13 @@
         <v>0</v>
       </c>
       <c r="D4" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E4" s="2">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F4" s="2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -983,7 +1006,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -994,13 +1017,13 @@
         <v>0</v>
       </c>
       <c r="D5" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E5" s="2">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F5" s="2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G5" s="3">
         <v>0</v>
@@ -1045,7 +1068,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -1056,13 +1079,13 @@
         <v>1</v>
       </c>
       <c r="D6" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E6" s="2">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F6" s="2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -1107,7 +1130,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -1118,13 +1141,13 @@
         <v>0</v>
       </c>
       <c r="D7" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E7" s="2">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F7" s="2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -1169,7 +1192,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -1180,13 +1203,13 @@
         <v>0</v>
       </c>
       <c r="D8" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E8" s="2">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F8" s="2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -1231,7 +1254,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>2</v>
       </c>
@@ -1242,13 +1265,13 @@
         <v>0</v>
       </c>
       <c r="D9" s="2">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E9" s="2">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="F9" s="2">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G9" s="3">
         <v>0</v>
@@ -1293,7 +1316,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>2</v>
       </c>
@@ -1304,13 +1327,13 @@
         <v>0</v>
       </c>
       <c r="D10" s="2">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E10" s="2">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="F10" s="2">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G10" s="3">
         <v>0</v>
@@ -1355,7 +1378,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>2</v>
       </c>
@@ -1366,13 +1389,13 @@
         <v>1</v>
       </c>
       <c r="D11" s="2">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E11" s="2">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="F11" s="2">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G11" s="3">
         <v>0</v>
@@ -1417,7 +1440,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>2</v>
       </c>
@@ -1428,13 +1451,13 @@
         <v>0</v>
       </c>
       <c r="D12" s="2">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E12" s="2">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="F12" s="2">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G12" s="3">
         <v>0</v>
@@ -1479,7 +1502,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>2</v>
       </c>
@@ -1490,13 +1513,13 @@
         <v>0</v>
       </c>
       <c r="D13" s="2">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E13" s="2">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="F13" s="2">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G13" s="3">
         <v>0</v>
@@ -1541,7 +1564,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>2</v>
       </c>
@@ -1552,13 +1575,13 @@
         <v>0</v>
       </c>
       <c r="D14" s="2">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E14" s="2">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="F14" s="2">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G14" s="3">
         <v>0</v>
@@ -1603,7 +1626,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>3</v>
       </c>
@@ -1623,13 +1646,13 @@
         <v>0</v>
       </c>
       <c r="G15" s="3">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H15" s="3">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="I15" s="3">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="J15" s="4">
         <v>1</v>
@@ -1665,7 +1688,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>3</v>
       </c>
@@ -1685,13 +1708,13 @@
         <v>0</v>
       </c>
       <c r="G16" s="3">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H16" s="3">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="I16" s="3">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="J16" s="4">
         <v>2</v>
@@ -1727,7 +1750,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>3</v>
       </c>
@@ -1747,13 +1770,13 @@
         <v>0</v>
       </c>
       <c r="G17" s="3">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H17" s="3">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="I17" s="3">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="J17" s="4">
         <v>0</v>
@@ -1789,7 +1812,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>3</v>
       </c>
@@ -1809,13 +1832,13 @@
         <v>0</v>
       </c>
       <c r="G18" s="3">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H18" s="3">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="I18" s="3">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="J18" s="4">
         <v>3</v>
@@ -1851,7 +1874,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>3</v>
       </c>
@@ -1871,13 +1894,13 @@
         <v>0</v>
       </c>
       <c r="G19" s="3">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H19" s="3">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="I19" s="3">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="J19" s="4">
         <v>2</v>
@@ -1913,7 +1936,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>3</v>
       </c>
@@ -1933,13 +1956,13 @@
         <v>0</v>
       </c>
       <c r="G20" s="3">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H20" s="3">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="I20" s="3">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="J20" s="4">
         <v>2</v>
@@ -1975,7 +1998,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>4</v>
       </c>
@@ -1995,13 +2018,13 @@
         <v>0</v>
       </c>
       <c r="G21" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H21" s="3">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="I21" s="3">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="J21" s="4">
         <v>3</v>
@@ -2037,7 +2060,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>4</v>
       </c>
@@ -2057,13 +2080,13 @@
         <v>0</v>
       </c>
       <c r="G22" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H22" s="3">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="I22" s="3">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="J22" s="4">
         <v>1</v>
@@ -2099,7 +2122,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>4</v>
       </c>
@@ -2119,13 +2142,13 @@
         <v>0</v>
       </c>
       <c r="G23" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H23" s="3">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="I23" s="3">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="J23" s="4">
         <v>1</v>
@@ -2161,7 +2184,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>4</v>
       </c>
@@ -2181,13 +2204,13 @@
         <v>0</v>
       </c>
       <c r="G24" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H24" s="3">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="I24" s="3">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="J24" s="4">
         <v>0</v>
@@ -2223,7 +2246,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>4</v>
       </c>
@@ -2243,13 +2266,13 @@
         <v>0</v>
       </c>
       <c r="G25" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H25" s="3">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="I25" s="3">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="J25" s="4">
         <v>2</v>
@@ -2285,7 +2308,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>4</v>
       </c>
@@ -2305,13 +2328,13 @@
         <v>0</v>
       </c>
       <c r="G26" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H26" s="3">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="I26" s="3">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="J26" s="4">
         <v>2</v>
@@ -2347,7 +2370,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>5</v>
       </c>
@@ -2409,7 +2432,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>5</v>
       </c>
@@ -2471,7 +2494,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>5</v>
       </c>
@@ -2533,7 +2556,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>5</v>
       </c>
@@ -2595,7 +2618,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>5</v>
       </c>
@@ -2657,7 +2680,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>5</v>
       </c>
@@ -2719,7 +2742,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>6</v>
       </c>
@@ -2781,7 +2804,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>6</v>
       </c>
@@ -2843,7 +2866,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>6</v>
       </c>
@@ -2905,7 +2928,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>6</v>
       </c>
@@ -2967,7 +2990,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>6</v>
       </c>
@@ -3029,7 +3052,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
data2 demand node 3 demand increased to distinguish objectives 2 & 3
</commit_message>
<xml_diff>
--- a/data2.xlsx
+++ b/data2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66129CC4-14F4-6743-8824-2D08A0056293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA0D4554-F554-A941-A21E-FAF8D92137D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="32200" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -225,7 +225,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -234,12 +234,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Uijt</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Uijt</t>
         </r>
       </text>
     </comment>
@@ -735,7 +744,7 @@
   <dimension ref="A1:V38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -890,10 +899,10 @@
         <v>4</v>
       </c>
       <c r="E3" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F3" s="2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -958,10 +967,10 @@
         <v>4</v>
       </c>
       <c r="E4" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F4" s="2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -1020,10 +1029,10 @@
         <v>4</v>
       </c>
       <c r="E5" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F5" s="2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G5" s="3">
         <v>0</v>
@@ -1044,13 +1053,13 @@
         <v>8</v>
       </c>
       <c r="M5" s="5">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="N5" s="5">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="O5" s="5">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="P5">
         <v>1</v>
@@ -1082,10 +1091,10 @@
         <v>4</v>
       </c>
       <c r="E6" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F6" s="2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -1144,10 +1153,10 @@
         <v>4</v>
       </c>
       <c r="E7" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F7" s="2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -1206,10 +1215,10 @@
         <v>4</v>
       </c>
       <c r="E8" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F8" s="2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -1268,10 +1277,10 @@
         <v>6</v>
       </c>
       <c r="E9" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F9" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G9" s="3">
         <v>0</v>
@@ -1330,10 +1339,10 @@
         <v>6</v>
       </c>
       <c r="E10" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F10" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G10" s="3">
         <v>0</v>
@@ -1392,10 +1401,10 @@
         <v>6</v>
       </c>
       <c r="E11" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F11" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G11" s="3">
         <v>0</v>
@@ -1454,10 +1463,10 @@
         <v>6</v>
       </c>
       <c r="E12" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F12" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G12" s="3">
         <v>0</v>
@@ -1516,10 +1525,10 @@
         <v>6</v>
       </c>
       <c r="E13" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F13" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G13" s="3">
         <v>0</v>
@@ -1578,10 +1587,10 @@
         <v>6</v>
       </c>
       <c r="E14" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F14" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G14" s="3">
         <v>0</v>
@@ -1646,7 +1655,7 @@
         <v>0</v>
       </c>
       <c r="G15" s="3">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="H15" s="3">
         <v>50</v>
@@ -1708,7 +1717,7 @@
         <v>0</v>
       </c>
       <c r="G16" s="3">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="H16" s="3">
         <v>50</v>
@@ -1770,7 +1779,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="3">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="H17" s="3">
         <v>50</v>
@@ -1832,7 +1841,7 @@
         <v>0</v>
       </c>
       <c r="G18" s="3">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="H18" s="3">
         <v>50</v>
@@ -1894,7 +1903,7 @@
         <v>0</v>
       </c>
       <c r="G19" s="3">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="H19" s="3">
         <v>50</v>
@@ -1956,7 +1965,7 @@
         <v>0</v>
       </c>
       <c r="G20" s="3">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="H20" s="3">
         <v>50</v>

</xml_diff>

<commit_message>
new data definition, scaling updated
</commit_message>
<xml_diff>
--- a/data2.xlsx
+++ b/data2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D19F4CD9-F8B8-4E46-87F2-DE94404022DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61ECA518-0FAE-E341-B59F-415063766C6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="32200" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2880" yWindow="2060" windowWidth="32200" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -176,7 +176,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -185,12 +185,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-djkt</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>djkt</t>
         </r>
       </text>
     </comment>
@@ -200,7 +209,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -209,12 +218,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Cijkt
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Cijkt
 </t>
         </r>
       </text>
@@ -282,7 +300,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -291,12 +309,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-bt</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>bt</t>
         </r>
       </text>
     </comment>
@@ -306,7 +333,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -315,12 +342,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-bt</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>bt</t>
         </r>
       </text>
     </comment>
@@ -744,7 +780,7 @@
   <dimension ref="A1:V38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -982,13 +1018,13 @@
         <v>0</v>
       </c>
       <c r="J4" s="4">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="K4" s="4">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="L4" s="4">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="M4" s="5">
         <v>5</v>
@@ -1044,19 +1080,19 @@
         <v>0</v>
       </c>
       <c r="J5" s="4">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="K5" s="4">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="L5" s="4">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="M5" s="5">
         <v>2</v>
       </c>
       <c r="N5" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O5" s="5">
         <v>2</v>
@@ -1124,13 +1160,13 @@
         <v>4</v>
       </c>
       <c r="P6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S6" s="6"/>
       <c r="T6" s="6"/>
@@ -1416,13 +1452,13 @@
         <v>0</v>
       </c>
       <c r="J11" s="4">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="K11" s="4">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="L11" s="4">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="M11" s="5">
         <v>1</v>
@@ -1434,13 +1470,13 @@
         <v>1</v>
       </c>
       <c r="P11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S11" s="6"/>
       <c r="T11" s="6"/>
@@ -2160,13 +2196,13 @@
         <v>12</v>
       </c>
       <c r="J23" s="4">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="K23" s="4">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="L23" s="4">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="M23" s="5">
         <v>8</v>
@@ -2532,13 +2568,13 @@
         <v>0</v>
       </c>
       <c r="J29" s="4">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="K29" s="4">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="L29" s="4">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="M29" s="5">
         <v>8</v>
@@ -2904,13 +2940,13 @@
         <v>0</v>
       </c>
       <c r="J35" s="4">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="K35" s="4">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="L35" s="4">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="M35" s="5">
         <v>8</v>

</xml_diff>